<commit_message>
Fix import file error in sonarcloud MU-265
</commit_message>
<xml_diff>
--- a/src/src/main/resources/templates/temp-import-groups.xlsx
+++ b/src/src/main/resources/templates/temp-import-groups.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hieu/Workspaces/current-work/mentorus/backend/src/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7CEF6C-0546-5A4E-A0B8-56FE9CFC2962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A132CE3A-B483-3A4C-AF83-7BF72218B653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -86,28 +86,12 @@
   </si>
   <si>
     <t>mentor@gmail.com</t>
-  </si>
-  <si>
-    <t>20127312@student.hcmus.edu.vn
-20127159@student.hcmus.edu.vn
-capybbv+1@gmail.com</t>
-  </si>
-  <si>
-    <t>capybbv+2@gmail.com</t>
-  </si>
-  <si>
-    <t>capybbv+teacher@gmail.com
-capybbv+teacher1@fitus.edu.vn</t>
-  </si>
-  <si>
-    <t>capybbv+teacher@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -198,9 +182,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -426,15 +407,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="8.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="10" width="25.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="10" width="39.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="10" width="28.33203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="10" width="20.5" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="10" width="27.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="4" width="17.5" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="4" width="21.1640625" collapsed="false"/>
-    <col min="9" max="26" customWidth="true" width="8.6640625" collapsed="false"/>
+    <col min="1" max="1" width="8.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="39" style="10" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="10" customWidth="1"/>
+    <col min="6" max="6" width="27" style="10" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" style="4" customWidth="1"/>
+    <col min="9" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1515,20 +1496,20 @@
   <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="4.5" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="28.5" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="46.5" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="16.6640625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="27.83203125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="23.83203125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="33.33203125" collapsed="false"/>
-    <col min="9" max="26" customWidth="true" width="9.1640625" collapsed="false"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" customWidth="1"/>
+    <col min="9" max="26" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1576,14 +1557,6 @@
       <c r="Z1" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" sqref="B4:B10001" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>"TEST,KTPM,Test import"</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="B2:B10001" allowBlank="false" errorStyle="stop" showDropDown="false">
-      <formula1>"TEST,KTPM,Test import"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>